<commit_message>
Nenhuma alteração  feita nos arquivos .doc e .xlsx, mas altera feita no cronograma
</commit_message>
<xml_diff>
--- a/Projeto/Tabela de Estimativa de Projeto Game_Shelf.xlsx
+++ b/Projeto/Tabela de Estimativa de Projeto Game_Shelf.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhuni\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garcia\Documents\GitHub\GameShelf_EVG\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
     <definedName name="TotalHorasProjeto">Geral!#REF!</definedName>
     <definedName name="UC">'RFS ou RFC'!$A$12:$C$27</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -710,7 +710,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1624,44 +1624,9 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1673,9 +1638,48 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1688,14 +1692,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1703,15 +1704,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2088,7 +2088,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2126,7 +2126,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2161,6 +2161,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2196,9 +2213,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2353,7 +2387,7 @@
   </sheetPr>
   <dimension ref="A3:AMK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -2370,75 +2404,75 @@
   <sheetData>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="114"/>
-      <c r="C4" s="114"/>
-      <c r="D4" s="114"/>
-      <c r="E4" s="114"/>
-      <c r="F4" s="114"/>
-      <c r="G4" s="114"/>
-      <c r="H4" s="114"/>
-      <c r="I4" s="114"/>
-      <c r="J4" s="114"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="115" t="s">
+      <c r="B6" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="115"/>
-      <c r="D6" s="116" t="s">
+      <c r="C6" s="103"/>
+      <c r="D6" s="104" t="s">
         <v>144</v>
       </c>
-      <c r="E6" s="116"/>
-      <c r="F6" s="116"/>
-      <c r="G6" s="116"/>
-      <c r="H6" s="116"/>
-      <c r="I6" s="116"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="104"/>
     </row>
     <row r="7" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="110"/>
-      <c r="D7" s="117" t="s">
+      <c r="C7" s="105"/>
+      <c r="D7" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="117"/>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
-      <c r="H7" s="117"/>
-      <c r="I7" s="117"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="106"/>
+      <c r="I7" s="106"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="109"/>
+      <c r="C8" s="107"/>
       <c r="D8" s="99">
         <v>42509</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="110" t="s">
+      <c r="F8" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="110"/>
-      <c r="H8" s="128">
+      <c r="G8" s="105"/>
+      <c r="H8" s="101">
         <v>1</v>
       </c>
       <c r="I8" s="3"/>
@@ -2446,25 +2480,25 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="108"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112"/>
-      <c r="G12" s="113" t="s">
+      <c r="C12" s="109"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="G12" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
       <c r="J12" s="5" t="s">
         <v>7</v>
       </c>
@@ -2474,20 +2508,20 @@
       <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="111" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
       <c r="E13" s="7">
         <f>Atores!D10+'RFS ou RFC'!D10</f>
         <v>132</v>
       </c>
-      <c r="G13" s="106" t="s">
+      <c r="G13" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
       <c r="J13" s="8">
         <f t="shared" ref="J13:J20" si="0">$E$13*$E$14*K13</f>
         <v>24.64</v>
@@ -2499,20 +2533,20 @@
       <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="112" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="107"/>
-      <c r="D14" s="107"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="112"/>
       <c r="E14" s="11">
         <f>dadoshistoricos!L30</f>
         <v>4</v>
       </c>
-      <c r="G14" s="104" t="s">
+      <c r="G14" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="113"/>
       <c r="J14" s="12">
         <f t="shared" si="0"/>
         <v>86.826666666666668</v>
@@ -2524,15 +2558,15 @@
       <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="108"/>
-      <c r="C15" s="108"/>
-      <c r="D15" s="108"/>
+      <c r="B15" s="114"/>
+      <c r="C15" s="114"/>
+      <c r="D15" s="114"/>
       <c r="F15"/>
-      <c r="G15" s="104" t="s">
+      <c r="G15" s="113" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="104"/>
-      <c r="I15" s="104"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
       <c r="J15" s="12">
         <f t="shared" si="0"/>
         <v>21.706666666666667</v>
@@ -2544,11 +2578,11 @@
       <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G16" s="104" t="s">
+      <c r="G16" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="104"/>
-      <c r="I16" s="104"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="113"/>
       <c r="J16" s="12">
         <f t="shared" si="0"/>
         <v>35.200000000000003</v>
@@ -2560,11 +2594,11 @@
       <c r="M16" s="10"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="G17" s="105" t="s">
+      <c r="G17" s="118" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="105"/>
-      <c r="I17" s="105"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
       <c r="J17" s="12">
         <f t="shared" si="0"/>
         <v>293.33333333333337</v>
@@ -2577,11 +2611,11 @@
       <c r="M17" s="6"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="G18" s="105" t="s">
+      <c r="G18" s="118" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="105"/>
-      <c r="I18" s="105"/>
+      <c r="H18" s="118"/>
+      <c r="I18" s="118"/>
       <c r="J18" s="12">
         <f t="shared" si="0"/>
         <v>11.733333333333334</v>
@@ -2593,11 +2627,11 @@
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="G19" s="105" t="s">
+      <c r="G19" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="105"/>
-      <c r="I19" s="105"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="118"/>
       <c r="J19" s="12">
         <f t="shared" si="0"/>
         <v>35.786666666666669</v>
@@ -2616,11 +2650,11 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="105" t="s">
+      <c r="G20" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="105"/>
-      <c r="I20" s="105"/>
+      <c r="H20" s="118"/>
+      <c r="I20" s="118"/>
       <c r="J20" s="12">
         <f t="shared" si="0"/>
         <v>18.773333333333333</v>
@@ -2632,11 +2666,11 @@
       <c r="L20" s="10"/>
     </row>
     <row r="21" spans="2:13" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="101" t="s">
+      <c r="G21" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="101"/>
-      <c r="I21" s="101"/>
+      <c r="H21" s="115"/>
+      <c r="I21" s="115"/>
       <c r="J21" s="16">
         <f>SUM(J13:J19)</f>
         <v>509.22666666666674</v>
@@ -2648,31 +2682,31 @@
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="116" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="102"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102"/>
-      <c r="H22" s="102"/>
-      <c r="I22" s="102"/>
-      <c r="J22" s="102"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="116"/>
+      <c r="F22" s="116"/>
+      <c r="G22" s="116"/>
+      <c r="H22" s="116"/>
+      <c r="I22" s="116"/>
+      <c r="J22" s="116"/>
       <c r="L22" s="10"/>
     </row>
     <row r="23" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="103" t="s">
+      <c r="B23" s="117" t="s">
         <v>110</v>
       </c>
-      <c r="C23" s="103"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="103"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="103"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
       <c r="L23" s="10"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
@@ -2697,37 +2731,21 @@
       <c r="L27" s="10"/>
     </row>
     <row r="28" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="103" t="s">
+      <c r="B28" s="117" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="103"/>
-      <c r="F28" s="103"/>
-      <c r="G28" s="103"/>
-      <c r="H28" s="103"/>
-      <c r="I28" s="103"/>
-      <c r="J28" s="103"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="117"/>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
     </row>
     <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B3:J4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="G15:I15"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="B22:J22"/>
     <mergeCell ref="B23:J23"/>
@@ -2737,6 +2755,22 @@
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="G19:I19"/>
     <mergeCell ref="G20:I20"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="B3:J4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -2782,11 +2816,11 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
       <c r="E2" s="19"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -3065,11 +3099,11 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
       <c r="E2" s="39"/>
       <c r="F2" s="39"/>
       <c r="G2" s="39"/>
@@ -3169,9 +3203,9 @@
       <c r="O10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="120"/>
-      <c r="B11" s="120"/>
-      <c r="C11" s="120"/>
+      <c r="A11" s="121"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="121"/>
       <c r="D11"/>
       <c r="O11"/>
     </row>
@@ -8440,12 +8474,12 @@
       <c r="M3"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="119"/>
+      <c r="E4" s="119"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
@@ -8484,12 +8518,12 @@
       <c r="M6"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="123" t="s">
+      <c r="B7" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" s="10"/>
@@ -8808,11 +8842,11 @@
       <c r="M21" s="10"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="122" t="s">
+      <c r="B22" s="123" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="122"/>
-      <c r="D22" s="122"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
       <c r="E22" s="60">
         <f>0.6+(0.01*SUM(D9*E9,D10*E10,D11*E11,D12*E12,D13*E13,D14*E14,D15*E15,D16*E16,D17*E17,D18*E18,D19*E19,D20*E20,D21*E21))</f>
         <v>0.90500000000000003</v>
@@ -8890,11 +8924,11 @@
       <c r="B28" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="121" t="s">
+      <c r="C28" s="126" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="121"/>
-      <c r="E28" s="121"/>
+      <c r="D28" s="126"/>
+      <c r="E28" s="126"/>
       <c r="F28" s="27">
         <v>1.5</v>
       </c>
@@ -8907,11 +8941,11 @@
       <c r="B29" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="121" t="s">
+      <c r="C29" s="126" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="126"/>
       <c r="F29" s="27">
         <v>0.5</v>
       </c>
@@ -8924,11 +8958,11 @@
       <c r="B30" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="121" t="s">
+      <c r="C30" s="126" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="121"/>
-      <c r="E30" s="121"/>
+      <c r="D30" s="126"/>
+      <c r="E30" s="126"/>
       <c r="F30" s="27">
         <v>1</v>
       </c>
@@ -8941,11 +8975,11 @@
       <c r="B31" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="121" t="s">
+      <c r="C31" s="126" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="121"/>
-      <c r="E31" s="121"/>
+      <c r="D31" s="126"/>
+      <c r="E31" s="126"/>
       <c r="F31" s="27">
         <v>0.5</v>
       </c>
@@ -8958,11 +8992,11 @@
       <c r="B32" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="121" t="s">
+      <c r="C32" s="126" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="121"/>
-      <c r="E32" s="121"/>
+      <c r="D32" s="126"/>
+      <c r="E32" s="126"/>
       <c r="F32" s="27">
         <v>1</v>
       </c>
@@ -8975,11 +9009,11 @@
       <c r="B33" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="121" t="s">
+      <c r="C33" s="126" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="121"/>
-      <c r="E33" s="121"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="126"/>
       <c r="F33" s="27">
         <v>2</v>
       </c>
@@ -8992,11 +9026,11 @@
       <c r="B34" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="121" t="s">
+      <c r="C34" s="126" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="121"/>
-      <c r="E34" s="121"/>
+      <c r="D34" s="126"/>
+      <c r="E34" s="126"/>
       <c r="F34" s="27">
         <v>-1</v>
       </c>
@@ -9009,11 +9043,11 @@
       <c r="B35" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C35" s="121" t="s">
+      <c r="C35" s="126" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="121"/>
-      <c r="E35" s="121"/>
+      <c r="D35" s="126"/>
+      <c r="E35" s="126"/>
       <c r="F35" s="27">
         <v>-1</v>
       </c>
@@ -9023,13 +9057,13 @@
       <c r="I35" s="59"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="122" t="s">
+      <c r="B36" s="123" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="122"/>
-      <c r="D36" s="122"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="122"/>
+      <c r="C36" s="123"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="123"/>
       <c r="G36" s="64">
         <f>1.4+(-0.03*SUM(F28*G28,F29*G29,F30*G30,F31*G31,F32*G32,F33*G33,F34*G34,F35*G35))</f>
         <v>1.2949999999999999</v>
@@ -9039,11 +9073,6 @@
   </sheetData>
   <sheetProtection password="C6D5" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="14">
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
@@ -9053,6 +9082,11 @@
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="C27:E27"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" showErrorMessage="1" promptTitle="Influência" sqref="E9:E21 I9:I21">
@@ -9093,19 +9127,19 @@
   <sheetData>
     <row r="1" spans="1:55" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="65"/>
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="127" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
       <c r="M1" s="66"/>
       <c r="N1" s="65"/>
       <c r="O1" s="65"/>
@@ -10900,10 +10934,10 @@
       <c r="G30" s="65"/>
       <c r="H30" s="65"/>
       <c r="I30" s="65"/>
-      <c r="J30" s="127" t="s">
+      <c r="J30" s="128" t="s">
         <v>107</v>
       </c>
-      <c r="K30" s="127"/>
+      <c r="K30" s="128"/>
       <c r="L30" s="87">
         <v>4</v>
       </c>

</xml_diff>